<commit_message>
Lab3 and Lab4 modified, defects screenshots added
</commit_message>
<xml_diff>
--- a/Lab3.xlsx
+++ b/Lab3.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="199">
   <si>
     <t xml:space="preserve">Название проекта</t>
   </si>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">Smoke</t>
   </si>
   <si>
-    <t xml:space="preserve">passed</t>
+    <t xml:space="preserve">not tested</t>
   </si>
   <si>
     <t xml:space="preserve">ФТ-10</t>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t xml:space="preserve">Нажать на подтверждение формы</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not passed</t>
   </si>
   <si>
     <r>
@@ -1031,7 +1028,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1059,7 +1056,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
-        <bgColor rgb="FFD6CFB7"/>
+        <bgColor rgb="FFB2B2B2"/>
       </patternFill>
     </fill>
     <fill>
@@ -1094,14 +1091,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF01C969"/>
-        <bgColor rgb="FF52A994"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FFBFBFBF"/>
       </patternFill>
     </fill>
     <fill>
@@ -1239,7 +1230,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1324,15 +1315,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="13" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="14" borderId="7" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="13" borderId="7" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1340,15 +1327,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="14" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="14" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="15" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="15" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="16" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1356,7 +1343,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="14" borderId="7" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="13" borderId="7" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1364,7 +1351,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="14" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1372,11 +1359,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="15" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="14" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="16" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="15" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1384,23 +1371,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="14" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="15" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="16" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="14" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="15" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="16" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1453,7 +1440,7 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF01C969"/>
+      <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFEBE7D9"/>
       <rgbColor rgb="FFBFE0D8"/>
       <rgbColor rgb="FFDCDCDC"/>
@@ -1463,12 +1450,12 @@
       <rgbColor rgb="FFF1CBA1"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF4BACC6"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFC3D69B"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FFC3D69B"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF52A994"/>
       <rgbColor rgb="FF003300"/>
@@ -1493,7 +1480,7 @@
       <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.45"/>
@@ -1578,10 +1565,10 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
@@ -1623,7 +1610,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="n">
         <v>1</v>
       </c>
@@ -1646,7 +1633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="n">
         <v>2</v>
       </c>
@@ -1669,7 +1656,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="n">
         <v>3</v>
       </c>
@@ -1692,7 +1679,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="n">
         <v>4</v>
       </c>
@@ -1715,7 +1702,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="n">
         <v>5</v>
       </c>
@@ -1738,7 +1725,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="n">
         <v>6</v>
       </c>
@@ -1757,8 +1744,8 @@
       <c r="F7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="20" t="s">
-        <v>34</v>
+      <c r="G7" s="18" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1766,16 +1753,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>36</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>37</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>23</v>
@@ -1795,7 +1782,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>32</v>
@@ -1807,7 +1794,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="n">
         <v>9</v>
       </c>
@@ -1818,10 +1805,10 @@
         <v>20</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>23</v>
@@ -1830,7 +1817,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="n">
         <v>10</v>
       </c>
@@ -1841,19 +1828,19 @@
         <v>20</v>
       </c>
       <c r="D11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="F11" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="21" t="s">
-        <v>41</v>
-      </c>
       <c r="G11" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="n">
         <v>11</v>
       </c>
@@ -1864,19 +1851,19 @@
         <v>20</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="21" t="s">
         <v>41</v>
       </c>
+      <c r="F12" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="G12" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="n">
         <v>12</v>
       </c>
@@ -1887,19 +1874,19 @@
         <v>20</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="G13" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="n">
         <v>13</v>
       </c>
@@ -1910,19 +1897,19 @@
         <v>20</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="n">
         <v>14</v>
       </c>
@@ -1933,13 +1920,13 @@
         <v>20</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>24</v>
@@ -1950,22 +1937,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="E16" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>49</v>
-      </c>
       <c r="F16" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="20" t="s">
-        <v>34</v>
+      <c r="G16" s="18" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1973,63 +1960,63 @@
         <v>16</v>
       </c>
       <c r="B17" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>48</v>
-      </c>
       <c r="E17" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="14" t="s">
+      <c r="E18" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>41</v>
+      <c r="F18" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="G18" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>55</v>
-      </c>
       <c r="F19" s="17" t="s">
         <v>23</v>
       </c>
@@ -2037,7 +2024,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="n">
         <v>19</v>
       </c>
@@ -2045,13 +2032,13 @@
         <v>19</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F20" s="17" t="s">
         <v>23</v>
@@ -2060,7 +2047,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="n">
         <v>20</v>
       </c>
@@ -2068,14 +2055,14 @@
         <v>25</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="16" t="s">
-        <v>58</v>
-      </c>
       <c r="F21" s="17" t="s">
         <v>23</v>
       </c>
@@ -2083,21 +2070,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="n">
         <v>21</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F22" s="17" t="s">
         <v>23</v>
@@ -2106,7 +2093,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="n">
         <v>22</v>
       </c>
@@ -2114,60 +2101,60 @@
         <v>25</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="13" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F23" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13" t="n">
-        <v>23</v>
-      </c>
-      <c r="B24" s="19" t="s">
+      <c r="C24" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="16" t="s">
+      <c r="F24" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="13" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" s="19" t="s">
+      <c r="C25" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="14" t="s">
+      <c r="E25" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="16" t="s">
-        <v>65</v>
-      </c>
       <c r="F25" s="17" t="s">
         <v>23</v>
       </c>
@@ -2175,18 +2162,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="n">
         <v>25</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E26" s="16" t="s">
         <v>32</v>
@@ -2203,13 +2190,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>33</v>
@@ -2217,26 +2204,26 @@
       <c r="F27" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="13" t="n">
         <v>27</v>
       </c>
       <c r="B28" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="14" t="s">
+      <c r="E28" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>68</v>
-      </c>
       <c r="F28" s="17" t="s">
         <v>23</v>
       </c>
@@ -2244,22 +2231,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>70</v>
-      </c>
       <c r="F29" s="17" t="s">
         <v>23</v>
       </c>
@@ -2267,21 +2254,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="n">
         <v>29</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="17" t="s">
         <v>23</v>
@@ -2290,22 +2277,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13" t="n">
         <v>30</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D31" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="16" t="s">
-        <v>72</v>
-      </c>
       <c r="F31" s="17" t="s">
         <v>23</v>
       </c>
@@ -2313,21 +2300,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="13" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F32" s="17" t="s">
         <v>23</v>
@@ -2336,7 +2323,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="13" t="n">
         <v>32</v>
       </c>
@@ -2344,13 +2331,13 @@
         <v>19</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F33" s="17" t="s">
         <v>23</v>
@@ -2359,7 +2346,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="13" t="n">
         <v>33</v>
       </c>
@@ -2367,13 +2354,13 @@
         <v>19</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F34" s="17" t="s">
         <v>23</v>
@@ -2387,25 +2374,25 @@
         <v>34</v>
       </c>
       <c r="B35" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" s="14" t="s">
+      <c r="E35" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="F35" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F35" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="13" t="n">
         <v>35</v>
       </c>
@@ -2413,13 +2400,13 @@
         <v>19</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F36" s="17" t="s">
         <v>23</v>
@@ -2428,21 +2415,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="13" t="n">
         <v>36</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F37" s="17" t="s">
         <v>23</v>
@@ -2451,7 +2438,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13" t="n">
         <v>37</v>
       </c>
@@ -2459,14 +2446,14 @@
         <v>19</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D38" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E38" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="E38" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="F38" s="17" t="s">
         <v>23</v>
       </c>
@@ -2474,7 +2461,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="13" t="n">
         <v>38</v>
       </c>
@@ -2482,13 +2469,13 @@
         <v>19</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F39" s="17" t="s">
         <v>23</v>
@@ -2497,7 +2484,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="13" t="n">
         <v>39</v>
       </c>
@@ -2505,13 +2492,13 @@
         <v>19</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F40" s="17" t="s">
         <v>23</v>
@@ -2520,7 +2507,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="13" t="n">
         <v>40</v>
       </c>
@@ -2528,13 +2515,13 @@
         <v>19</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F41" s="17" t="s">
         <v>23</v>
@@ -2543,22 +2530,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="13" t="n">
         <v>41</v>
       </c>
       <c r="B42" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>86</v>
-      </c>
       <c r="F42" s="17" t="s">
         <v>23</v>
       </c>
@@ -2566,21 +2553,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="13" t="n">
         <v>42</v>
       </c>
       <c r="B43" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="15" t="s">
         <v>87</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>88</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F43" s="17" t="s">
         <v>23</v>
@@ -2589,21 +2576,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="13" t="n">
         <v>43</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F44" s="17" t="s">
         <v>23</v>
@@ -2612,7 +2599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="13" t="n">
         <v>44</v>
       </c>
@@ -2620,13 +2607,13 @@
         <v>25</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F45" s="17" t="s">
         <v>23</v>
@@ -2635,22 +2622,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="13" t="n">
         <v>45</v>
       </c>
       <c r="B46" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D46" s="19" t="s">
+      <c r="E46" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="16" t="s">
-        <v>95</v>
-      </c>
       <c r="F46" s="17" t="s">
         <v>23</v>
       </c>
@@ -2658,21 +2645,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="13" t="n">
         <v>46</v>
       </c>
       <c r="B47" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C47" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>94</v>
-      </c>
       <c r="E47" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>23</v>
@@ -2681,22 +2668,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="13" t="n">
         <v>47</v>
       </c>
       <c r="B48" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="E48" s="16" t="s">
-        <v>98</v>
-      </c>
       <c r="F48" s="17" t="s">
         <v>23</v>
       </c>
@@ -2704,7 +2691,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="13" t="n">
         <v>48</v>
       </c>
@@ -2712,14 +2699,14 @@
         <v>19</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D49" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E49" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="E49" s="16" t="s">
-        <v>100</v>
-      </c>
       <c r="F49" s="17" t="s">
         <v>23</v>
       </c>
@@ -2727,7 +2714,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="13" t="n">
         <v>49</v>
       </c>
@@ -2735,13 +2722,13 @@
         <v>19</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E50" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F50" s="17" t="s">
         <v>23</v>
@@ -2769,10 +2756,10 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.9"/>
@@ -2784,740 +2771,740 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="26" t="s">
+      <c r="F2" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="G2" s="27"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="28"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="30" t="s">
+      <c r="C3" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="32" t="s">
+      <c r="E3" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="F3" s="33"/>
+      <c r="G3" s="34"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="36" t="s">
+      <c r="F4" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="37"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" s="38"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="29"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="36" t="s">
+      <c r="F5" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="G5" s="37"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="G5" s="38"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="36" t="s">
+      <c r="F6" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="G6" s="37"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="G6" s="38"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="29"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="36" t="s">
+      <c r="F7" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="G7" s="37"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="G7" s="38"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="36" t="s">
+      <c r="F8" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="G8" s="37"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="G8" s="38"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="36" t="s">
+      <c r="F9" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="G9" s="37"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="38"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="36" t="s">
+      <c r="F10" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="G10" s="37"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="G10" s="38"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="36" t="s">
+      <c r="F11" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="F11" s="37" t="s">
+      <c r="G11" s="37"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="G11" s="38"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="36" t="s">
+      <c r="F12" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="G12" s="37"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="G12" s="38"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="36" t="s">
+      <c r="F13" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="G13" s="37"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="G13" s="38"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="29"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="36" t="s">
+      <c r="F14" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="G14" s="37"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="G14" s="38"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="29"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="39" t="s">
+      <c r="F15" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="G15" s="40"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G15" s="41"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="32" t="s">
+      <c r="E16" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="F16" s="33"/>
+      <c r="G16" s="34"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="28"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="F16" s="34"/>
-      <c r="G16" s="35"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="29"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="36" t="s">
+      <c r="F17" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="F17" s="37" t="s">
+      <c r="G17" s="37"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="28"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="G17" s="38"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="29"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="36" t="s">
+      <c r="F18" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="G18" s="37"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="28"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="G18" s="38"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="29"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="36" t="s">
+      <c r="F19" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="F19" s="37" t="s">
+      <c r="G19" s="37"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="28"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="G19" s="38"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="29"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="39" t="s">
+      <c r="F20" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="F20" s="40" t="s">
+      <c r="G20" s="40"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="28" t="n">
+        <v>4</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="G20" s="41"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="29" t="n">
-        <v>4</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="32" t="s">
+      <c r="E21" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="F21" s="33"/>
+      <c r="G21" s="34"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="28"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="35"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="29"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="36" t="s">
+      <c r="F22" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="F22" s="37" t="s">
+      <c r="G22" s="37"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="28"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="G22" s="38"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="29"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="36" t="s">
+      <c r="F23" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="F23" s="37" t="s">
+      <c r="G23" s="37"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="28"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="G24" s="37"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="28"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="G23" s="38"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="29"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="36" t="s">
-        <v>140</v>
-      </c>
-      <c r="F24" s="37" t="s">
-        <v>141</v>
-      </c>
-      <c r="G24" s="38"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="29"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="39" t="s">
+      <c r="F25" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="G25" s="40"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="28" t="n">
+        <v>5</v>
+      </c>
+      <c r="B26" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="F25" s="40" t="s">
-        <v>143</v>
-      </c>
-      <c r="G25" s="41"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="29" t="n">
-        <v>5</v>
-      </c>
-      <c r="B26" s="30" t="s">
+      <c r="C26" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="C26" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26" s="32" t="s">
+      <c r="E26" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="F26" s="33"/>
+      <c r="G26" s="34"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="35"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="29"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="36" t="s">
+      <c r="F27" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="G27" s="37"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="F27" s="37" t="s">
-        <v>147</v>
-      </c>
-      <c r="G27" s="38"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="29"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="36" t="s">
+      <c r="F28" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="F28" s="37" t="s">
+      <c r="G28" s="37"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="G28" s="38"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="29"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="36" t="s">
+      <c r="F29" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="F29" s="37" t="s">
+      <c r="G29" s="37"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="G29" s="38"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="29"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="36" t="s">
+      <c r="F30" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="F30" s="37" t="s">
+      <c r="G30" s="37"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="G30" s="38"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="29"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="39" t="s">
+      <c r="F31" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="F31" s="40" t="s">
+      <c r="G31" s="40"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="28" t="n">
+        <v>6</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="G31" s="41"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="29" t="n">
-        <v>6</v>
-      </c>
-      <c r="B32" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="D32" s="32" t="s">
+      <c r="E32" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="F32" s="33"/>
+      <c r="G32" s="34"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="28"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="29"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="36" t="s">
+      <c r="F33" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="G33" s="37"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="28"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="F33" s="37" t="s">
-        <v>147</v>
-      </c>
-      <c r="G33" s="38"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="29"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="36" t="s">
+      <c r="F34" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="F34" s="37" t="s">
+      <c r="G34" s="37"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="28"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="G34" s="38"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="29"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="36" t="s">
+      <c r="F35" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="F35" s="37" t="s">
+      <c r="G35" s="37"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="28"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="G35" s="38"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="29"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="36" t="s">
+      <c r="F36" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="F36" s="37" t="s">
+      <c r="G36" s="37"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="28"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="G36" s="38"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="29"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="36" t="s">
+      <c r="F37" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="F37" s="37" t="s">
+      <c r="G37" s="37"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="28"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="G37" s="38"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="29"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="36" t="s">
+      <c r="F38" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="F38" s="37" t="s">
+      <c r="G38" s="37"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="28"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="G38" s="38"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="29"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="36" t="s">
+      <c r="F39" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="F39" s="37" t="s">
+      <c r="G39" s="37"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="28"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="G39" s="38"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="29"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="36" t="s">
+      <c r="F40" s="36" t="s">
         <v>178</v>
       </c>
-      <c r="F40" s="37" t="s">
+      <c r="G40" s="37"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="28"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="G40" s="38"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="29"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="36" t="s">
+      <c r="F41" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="F41" s="37" t="s">
+      <c r="G41" s="37"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="28"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="G41" s="38"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="29"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="39" t="s">
+      <c r="F42" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="F42" s="40" t="s">
+      <c r="G42" s="40"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="28" t="n">
+        <v>7</v>
+      </c>
+      <c r="B43" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="G42" s="41"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="29" t="n">
-        <v>7</v>
-      </c>
-      <c r="B43" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="D43" s="32" t="s">
+      <c r="E43" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="E43" s="33" t="s">
+      <c r="F43" s="33"/>
+      <c r="G43" s="34"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="28"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="35" t="s">
         <v>185</v>
       </c>
-      <c r="F43" s="34"/>
-      <c r="G43" s="35"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="29"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="36" t="s">
+      <c r="F44" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="F44" s="37" t="s">
+      <c r="G44" s="37"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="28"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="G44" s="38"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="29"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="36" t="s">
+      <c r="F45" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="F45" s="37" t="s">
+      <c r="G45" s="37"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="28"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="G45" s="38"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="29"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="36" t="s">
+      <c r="F46" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="F46" s="37" t="s">
+      <c r="G46" s="37"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="28"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="G46" s="38"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="29"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="39" t="s">
+      <c r="F47" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="F47" s="40" t="s">
+      <c r="G47" s="40"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="28" t="n">
+        <v>8</v>
+      </c>
+      <c r="B48" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="E48" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="G47" s="41"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="29" t="n">
-        <v>8</v>
-      </c>
-      <c r="B48" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="C48" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="D48" s="32" t="s">
-        <v>184</v>
-      </c>
-      <c r="E48" s="33" t="s">
+      <c r="F48" s="33"/>
+      <c r="G48" s="34"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="28"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="F48" s="34"/>
-      <c r="G48" s="35"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="29"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="36" t="s">
+      <c r="F49" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="G49" s="37"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="28"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="35" t="s">
         <v>195</v>
       </c>
-      <c r="F49" s="37" t="s">
-        <v>187</v>
-      </c>
-      <c r="G49" s="38"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="29"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="36" t="s">
+      <c r="F50" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="G50" s="37"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="28"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="F50" s="37" t="s">
-        <v>189</v>
-      </c>
-      <c r="G50" s="38"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="29"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="36" t="s">
+      <c r="F51" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="F51" s="37" t="s">
+      <c r="G51" s="37"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="28"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="G51" s="38"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="29"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="F52" s="40" t="s">
-        <v>193</v>
-      </c>
-      <c r="G52" s="41"/>
+      <c r="F52" s="39" t="s">
+        <v>192</v>
+      </c>
+      <c r="G52" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="28">

</xml_diff>